<commit_message>
Atlas.ti as text. Text fixes to tooltips
</commit_message>
<xml_diff>
--- a/app/data/Refined Features checklist.xlsx
+++ b/app/data/Refined Features checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="refined" sheetId="1" state="visible" r:id="rId2"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="447">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -99,10 +99,10 @@
     <t xml:space="preserve">Image files (bmp, jpg, png, ewmf)</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Survey Platform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference Management Tools</t>
+    <t xml:space="preserve">Web survey platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference management tools</t>
   </si>
   <si>
     <t xml:space="preserve">Email sources</t>
@@ -111,9 +111,15 @@
     <t xml:space="preserve">Social media</t>
   </si>
   <si>
+    <t xml:space="preserve">Import from ODBC databases</t>
+  </si>
+  <si>
     <t xml:space="preserve">Importation from ODBC databases</t>
   </si>
   <si>
+    <t xml:space="preserve">Import from PowerPoint</t>
+  </si>
+  <si>
     <t xml:space="preserve">Importation of Powerpoint</t>
   </si>
   <si>
@@ -153,7 +159,7 @@
     <t xml:space="preserve">Reports</t>
   </si>
   <si>
-    <t xml:space="preserve">Video/audio excerpting</t>
+    <t xml:space="preserve">Video/Audio Excerpting</t>
   </si>
   <si>
     <t xml:space="preserve">Import, excerpt, and sync transcripts to video and audio</t>
@@ -171,7 +177,7 @@
     <t xml:space="preserve">Sorting your media files, customizing column views, and filtering by sub-group using Boolean operators</t>
   </si>
   <si>
-    <t xml:space="preserve">Case/document management</t>
+    <t xml:space="preserve">Case/Document Management</t>
   </si>
   <si>
     <t xml:space="preserve">Add/delete cases</t>
@@ -216,7 +222,7 @@
     <t xml:space="preserve">Rotating and resizing images</t>
   </si>
   <si>
-    <t xml:space="preserve">Memo system</t>
+    <t xml:space="preserve">Memo System</t>
   </si>
   <si>
     <t xml:space="preserve">Create, edit, delete, sort memos</t>
@@ -344,7 +350,7 @@
     <t xml:space="preserve">Resize codes</t>
   </si>
   <si>
-    <t xml:space="preserve">Code overview/ color codes</t>
+    <t xml:space="preserve">Code overview/color codes</t>
   </si>
   <si>
     <t xml:space="preserve">Get overview of coded segments/frequencies</t>
@@ -428,7 +434,7 @@
     <t xml:space="preserve">Coding by variable</t>
   </si>
   <si>
-    <t xml:space="preserve">Code Weight/Rating system</t>
+    <t xml:space="preserve">Code weight/Rating system</t>
   </si>
   <si>
     <t xml:space="preserve">Overlay a numerical dimension onto your commonly coded qualitative data
@@ -453,10 +459,10 @@
     <t xml:space="preserve">Sentiment Analysis</t>
   </si>
   <si>
-    <t xml:space="preserve">Analyze the tone of the docment/case and determine if it is negative, neutral, or positive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stopword Removal (in frequency analysis)</t>
+    <t xml:space="preserve">Analyze the tone of the document/case and determine if it is negative, neutral, or positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stopword removal (in frequency analysis)</t>
   </si>
   <si>
     <t xml:space="preserve">Remove "noise" word like at, a, the…</t>
@@ -519,7 +525,7 @@
     <t xml:space="preserve">Work with operating systems and other tools (databases, excel, etc.)</t>
   </si>
   <si>
-    <t xml:space="preserve">Open Import/Export Migration</t>
+    <t xml:space="preserve">Open import/Export migration</t>
   </si>
   <si>
     <t xml:space="preserve">Import any data format and any software file (SurveyMonkey, NVivo, Atlas.ti, MaxQDA, Saturate, HyperResearch, Quirkos, Excel, Word...)
@@ -607,7 +613,7 @@
     <t xml:space="preserve">Accessibility</t>
   </si>
   <si>
-    <t xml:space="preserve">Good User Interface</t>
+    <t xml:space="preserve">Good user interface</t>
   </si>
   <si>
     <t xml:space="preserve">Intuitive interface and design</t>
@@ -626,7 +632,13 @@
     <t xml:space="preserve">Command log/Inter-coders agreement analysis</t>
   </si>
   <si>
+    <t xml:space="preserve">Training center</t>
+  </si>
+  <si>
     <t xml:space="preserve">Training Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding agreement</t>
   </si>
   <si>
     <t xml:space="preserve">Coding Agreement</t>
@@ -750,7 +762,7 @@
     <t xml:space="preserve">Free assistance in converting your projects in other products, like NVivo, Atlas.ti, MaxQDA, HyperResearch, Saturate, and Excel, to Dedoose</t>
   </si>
   <si>
-    <t xml:space="preserve">Free Technical support</t>
+    <t xml:space="preserve">Free technical support</t>
   </si>
   <si>
     <t xml:space="preserve">Online/by phone</t>
@@ -759,7 +771,7 @@
     <t xml:space="preserve">Data Collection</t>
   </si>
   <si>
-    <t xml:space="preserve">Mobile Application for Data Collection</t>
+    <t xml:space="preserve">Mobile application for data collection</t>
   </si>
   <si>
     <t xml:space="preserve">Can collect data through a mobile application</t>
@@ -771,7 +783,7 @@
     <t xml:space="preserve">Note Taking</t>
   </si>
   <si>
-    <t xml:space="preserve">Import from Collection Application</t>
+    <t xml:space="preserve">Import from collection application</t>
   </si>
   <si>
     <t xml:space="preserve">Can import from collection application</t>
@@ -792,6 +804,12 @@
     <t xml:space="preserve">MS Word, RTF, Plain txt, HTML</t>
   </si>
   <si>
+    <t xml:space="preserve">Web Survey Platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference Management Tools</t>
+  </si>
+  <si>
     <t xml:space="preserve">memos</t>
   </si>
   <si>
@@ -816,6 +834,9 @@
     <t xml:space="preserve">Use pre-defined reports or create your own using a Wizard. Save reports and share with others.</t>
   </si>
   <si>
+    <t xml:space="preserve">Video/audio excerpting</t>
+  </si>
+  <si>
     <t xml:space="preserve">import, excerpt, and sync transcripts to video and audio</t>
   </si>
   <si>
@@ -853,6 +874,9 @@
   </si>
   <si>
     <t xml:space="preserve">image rotation and resizing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo system</t>
   </si>
   <si>
     <t xml:space="preserve">create, edit, delete, sort</t>
@@ -1013,6 +1037,9 @@
     <t xml:space="preserve">identify recurring sequences of codes. This feature can produce frequency lists of all sequences involving two selected sets of codes as well as the percentage of times one code follows or is followed by another one; (heatmap, correspondence analysis, correlation, chi-sqare)</t>
   </si>
   <si>
+    <t xml:space="preserve">Code Weight/Rating system</t>
+  </si>
+  <si>
     <t xml:space="preserve">overlay a numerical dimension onto your commonly coded qualitative data
 </t>
   </si>
@@ -1038,6 +1065,9 @@
     <t xml:space="preserve">Use Automated Analysis of Themes and Sentiment to automatically discover emerging themes and sentiment within your data in a matter of minutes</t>
   </si>
   <si>
+    <t xml:space="preserve">Stopword Removal (in frequency analysis)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lemmitization (in frequency analysis)</t>
   </si>
   <si>
@@ -1153,6 +1183,9 @@
     <t xml:space="preserve">whole project exportation</t>
   </si>
   <si>
+    <t xml:space="preserve">Good User Interface</t>
+  </si>
+  <si>
     <t xml:space="preserve">Good interface or Good Design</t>
   </si>
   <si>
@@ -1350,7 +1383,16 @@
     <t xml:space="preserve">these projects are directly importable into your Dedoose workspace</t>
   </si>
   <si>
+    <t xml:space="preserve">Free Technical support</t>
+  </si>
+  <si>
     <t xml:space="preserve">online/by phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile Application for Data Collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Import from Collection Application</t>
   </si>
   <si>
     <t xml:space="preserve">Miscellaneous features</t>
@@ -2265,19 +2307,19 @@
   <dimension ref="A1:V267"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A27" activeCellId="0" sqref="A27:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.5627530364373"/>
     <col collapsed="false" hidden="false" max="11" min="4" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="17" min="12" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2748,7 +2790,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="12" t="n">
         <v>1</v>
@@ -2791,10 +2833,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" s="12" t="n">
         <v>0</v>
@@ -2837,10 +2879,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D13" s="12" t="n">
         <v>1</v>
@@ -2883,10 +2925,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D14" s="12" t="n">
         <v>0</v>
@@ -2929,10 +2971,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D15" s="12" t="n">
         <v>0</v>
@@ -2975,10 +3017,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D16" s="12" t="n">
         <v>1</v>
@@ -3021,9 +3063,11 @@
         <v>11</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>29</v>
+      </c>
       <c r="D17" s="12" t="n">
         <v>1</v>
       </c>
@@ -3057,10 +3101,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D18" s="12" t="n">
         <v>0</v>
@@ -3103,10 +3147,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D19" s="12" t="n">
         <v>0</v>
@@ -3149,10 +3193,10 @@
         <v>11</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D20" s="12" t="n">
         <v>1</v>
@@ -3195,10 +3239,10 @@
         <v>11</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D21" s="12" t="n">
         <v>1</v>
@@ -3262,13 +3306,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D23" s="28" t="n">
         <v>1</v>
@@ -3308,10 +3352,10 @@
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="28" t="n">
@@ -3352,13 +3396,13 @@
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D25" s="28" t="n">
         <v>0</v>
@@ -3422,13 +3466,13 @@
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D27" s="12" t="n">
         <v>1</v>
@@ -3468,13 +3512,13 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D28" s="12" t="n">
         <v>1</v>
@@ -3514,13 +3558,13 @@
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D29" s="12" t="n">
         <v>1</v>
@@ -3560,13 +3604,13 @@
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D30" s="12" t="n">
         <v>1</v>
@@ -3606,13 +3650,13 @@
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D31" s="12" t="n">
         <v>1</v>
@@ -3652,13 +3696,13 @@
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D32" s="12" t="n">
         <v>1</v>
@@ -3698,13 +3742,13 @@
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D33" s="12" t="n">
         <v>1</v>
@@ -3768,13 +3812,13 @@
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D35" s="12" t="n">
         <v>1</v>
@@ -3814,13 +3858,13 @@
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D36" s="12" t="n">
         <v>1</v>
@@ -3884,13 +3928,13 @@
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D38" s="12" t="n">
         <v>1</v>
@@ -3930,13 +3974,13 @@
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="13" t="n">
@@ -3974,13 +4018,13 @@
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D40" s="12" t="n">
         <v>1</v>
@@ -4020,13 +4064,13 @@
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D41" s="12" t="n">
         <v>1</v>
@@ -4066,13 +4110,13 @@
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D42" s="12" t="n">
         <v>1</v>
@@ -4112,10 +4156,10 @@
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="12" t="n">
@@ -4156,13 +4200,13 @@
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D44" s="12" t="n">
         <v>1</v>
@@ -4202,13 +4246,13 @@
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D45" s="12" t="n">
         <v>1</v>
@@ -4248,13 +4292,13 @@
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D46" s="12" t="n">
         <v>0</v>
@@ -4290,13 +4334,13 @@
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D47" s="12" t="n">
         <v>0</v>
@@ -4360,13 +4404,13 @@
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D49" s="12" t="n">
         <v>1</v>
@@ -4406,13 +4450,13 @@
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D50" s="12" t="n">
         <v>1</v>
@@ -4452,13 +4496,13 @@
     </row>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D51" s="12" t="n">
         <v>1</v>
@@ -4498,13 +4542,13 @@
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D52" s="12" t="n">
         <v>1</v>
@@ -4544,13 +4588,13 @@
     </row>
     <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D53" s="12" t="n">
         <v>0</v>
@@ -4590,13 +4634,13 @@
     </row>
     <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D54" s="12" t="n">
         <v>1</v>
@@ -4636,13 +4680,13 @@
     </row>
     <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D55" s="12" t="n">
         <v>0</v>
@@ -4682,13 +4726,13 @@
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D56" s="12" t="n">
         <v>1</v>
@@ -4728,13 +4772,13 @@
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D57" s="12" t="n">
         <v>0</v>
@@ -4774,13 +4818,13 @@
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D58" s="12" t="n">
         <v>1</v>
@@ -4820,13 +4864,13 @@
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D59" s="12" t="n">
         <v>0</v>
@@ -4866,13 +4910,13 @@
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D60" s="12" t="n">
         <v>1</v>
@@ -4912,13 +4956,13 @@
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D61" s="12" t="n">
         <v>0</v>
@@ -4958,13 +5002,13 @@
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D62" s="12" t="n">
         <v>0</v>
@@ -5028,13 +5072,13 @@
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D64" s="12" t="n">
         <v>1</v>
@@ -5074,13 +5118,13 @@
     </row>
     <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D65" s="12" t="n">
         <v>1</v>
@@ -5120,13 +5164,13 @@
     </row>
     <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D66" s="12" t="n">
         <v>1</v>
@@ -5166,13 +5210,13 @@
     </row>
     <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D67" s="12" t="n">
         <v>0</v>
@@ -5212,13 +5256,13 @@
     </row>
     <row r="68" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D68" s="12" t="n">
         <v>1</v>
@@ -5258,13 +5302,13 @@
     </row>
     <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D69" s="12" t="n">
         <v>0</v>
@@ -5304,13 +5348,13 @@
     </row>
     <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D70" s="12" t="n">
         <v>0</v>
@@ -5350,13 +5394,13 @@
     </row>
     <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B71" s="24" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D71" s="12" t="n">
         <v>1</v>
@@ -5396,13 +5440,13 @@
     </row>
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D72" s="12" t="n">
         <v>1</v>
@@ -5442,13 +5486,13 @@
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D73" s="12" t="n">
         <v>1</v>
@@ -5488,13 +5532,13 @@
     </row>
     <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B74" s="38" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D74" s="39" t="n">
         <v>1</v>
@@ -5534,13 +5578,13 @@
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D75" s="12" t="n">
         <v>0</v>
@@ -5604,13 +5648,13 @@
     </row>
     <row r="77" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B77" s="47" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D77" s="48" t="n">
         <v>1</v>
@@ -5650,13 +5694,13 @@
     </row>
     <row r="78" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D78" s="12" t="n">
         <v>0</v>
@@ -5696,13 +5740,13 @@
     </row>
     <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B79" s="47" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D79" s="48" t="n">
         <v>1</v>
@@ -5742,13 +5786,13 @@
     </row>
     <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B80" s="24" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D80" s="12" t="n">
         <v>1</v>
@@ -5788,13 +5832,13 @@
     </row>
     <row r="81" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B81" s="24" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C81" s="34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D81" s="12" t="n">
         <v>0</v>
@@ -5834,13 +5878,13 @@
     </row>
     <row r="82" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B82" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D82" s="12" t="n">
         <v>1</v>
@@ -5880,13 +5924,13 @@
     </row>
     <row r="83" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B83" s="47" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D83" s="48" t="n">
         <v>1</v>
@@ -5926,13 +5970,13 @@
     </row>
     <row r="84" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D84" s="12" t="n">
         <v>1</v>
@@ -5972,13 +6016,13 @@
     </row>
     <row r="85" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B85" s="24" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D85" s="12" t="n">
         <v>1</v>
@@ -6018,13 +6062,13 @@
     </row>
     <row r="86" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D86" s="12" t="n">
         <v>0</v>
@@ -6064,13 +6108,13 @@
     </row>
     <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B87" s="24" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D87" s="12" t="n">
         <v>0</v>
@@ -6110,13 +6154,13 @@
     </row>
     <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D88" s="12" t="n">
         <v>0</v>
@@ -6156,13 +6200,13 @@
     </row>
     <row r="89" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B89" s="24" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D89" s="12" t="n">
         <v>0</v>
@@ -6198,13 +6242,13 @@
     </row>
     <row r="90" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B90" s="47" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D90" s="48" t="n">
         <v>1</v>
@@ -6268,13 +6312,13 @@
     </row>
     <row r="92" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B92" s="24" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D92" s="12" t="n">
         <v>1</v>
@@ -6314,13 +6358,13 @@
     </row>
     <row r="93" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B93" s="24" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D93" s="12" t="n">
         <v>1</v>
@@ -6360,13 +6404,13 @@
     </row>
     <row r="94" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B94" s="24" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D94" s="12" t="n">
         <v>1</v>
@@ -6406,13 +6450,13 @@
     </row>
     <row r="95" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B95" s="24" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D95" s="12" t="n">
         <v>1</v>
@@ -6476,13 +6520,13 @@
     </row>
     <row r="97" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B97" s="24" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D97" s="12" t="n">
         <v>0</v>
@@ -6522,13 +6566,13 @@
     </row>
     <row r="98" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B98" s="24" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D98" s="12" t="n">
         <v>0</v>
@@ -6568,13 +6612,13 @@
     </row>
     <row r="99" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B99" s="24" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D99" s="12" t="n">
         <v>1</v>
@@ -6614,13 +6658,13 @@
     </row>
     <row r="100" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B100" s="24" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D100" s="12" t="n">
         <v>0</v>
@@ -6684,13 +6728,13 @@
     </row>
     <row r="102" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B102" s="24" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D102" s="12" t="n">
         <v>1</v>
@@ -6730,13 +6774,13 @@
     </row>
     <row r="103" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B103" s="24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C103" s="34" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D103" s="12" t="n">
         <v>0</v>
@@ -6800,13 +6844,13 @@
     </row>
     <row r="105" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B105" s="24" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D105" s="12" t="n">
         <v>1</v>
@@ -6846,13 +6890,13 @@
     </row>
     <row r="106" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B106" s="24" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D106" s="12" t="n">
         <v>1</v>
@@ -6892,13 +6936,13 @@
     </row>
     <row r="107" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D107" s="12" t="n">
         <v>0</v>
@@ -6938,13 +6982,13 @@
     </row>
     <row r="108" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D108" s="12" t="n">
         <v>0</v>
@@ -6984,13 +7028,13 @@
     </row>
     <row r="109" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D109" s="12" t="n">
         <v>0</v>
@@ -7030,13 +7074,13 @@
     </row>
     <row r="110" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D110" s="12" t="n">
         <v>1</v>
@@ -7076,13 +7120,13 @@
     </row>
     <row r="111" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D111" s="12" t="n">
         <v>1</v>
@@ -7122,13 +7166,13 @@
     </row>
     <row r="112" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D112" s="12" t="n">
         <v>0</v>
@@ -7168,13 +7212,13 @@
     </row>
     <row r="113" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D113" s="12" t="n">
         <v>0</v>
@@ -7214,13 +7258,13 @@
     </row>
     <row r="114" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D114" s="12" t="n">
         <v>0</v>
@@ -7260,13 +7304,13 @@
     </row>
     <row r="115" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D115" s="12" t="n">
         <v>1</v>
@@ -7306,13 +7350,13 @@
     </row>
     <row r="116" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D116" s="12" t="n">
         <v>1</v>
@@ -7352,13 +7396,13 @@
     </row>
     <row r="117" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D117" s="12" t="n">
         <v>0</v>
@@ -7398,13 +7442,13 @@
     </row>
     <row r="118" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D118" s="12" t="n">
         <v>1</v>
@@ -7444,13 +7488,13 @@
     </row>
     <row r="119" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B119" s="24" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D119" s="12" t="n">
         <v>1</v>
@@ -7490,13 +7534,13 @@
     </row>
     <row r="120" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B120" s="24" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D120" s="12" t="n">
         <v>1</v>
@@ -7536,13 +7580,13 @@
     </row>
     <row r="121" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B121" s="24" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D121" s="12" t="n">
         <v>1</v>
@@ -7582,10 +7626,10 @@
     </row>
     <row r="122" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B122" s="24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="12" t="n">
@@ -7626,13 +7670,13 @@
     </row>
     <row r="123" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B123" s="24" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D123" s="12" t="n">
         <v>1</v>
@@ -7672,13 +7716,13 @@
     </row>
     <row r="124" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B124" s="24" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D124" s="12" t="n">
         <v>1</v>
@@ -7718,13 +7762,13 @@
     </row>
     <row r="125" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B125" s="24" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D125" s="12" t="n">
         <v>0</v>
@@ -7764,13 +7808,13 @@
     </row>
     <row r="126" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B126" s="24" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D126" s="12" t="n">
         <v>0</v>
@@ -7834,13 +7878,13 @@
     </row>
     <row r="128" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="22" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B128" s="24" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D128" s="12" t="n">
         <v>1</v>
@@ -7880,13 +7924,13 @@
     </row>
     <row r="129" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="22" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B129" s="38" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C129" s="34" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D129" s="39" t="n">
         <v>1</v>
@@ -7950,13 +7994,13 @@
     </row>
     <row r="131" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="50" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B131" s="24" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D131" s="12" t="n">
         <v>0</v>
@@ -7996,13 +8040,13 @@
     </row>
     <row r="132" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="50" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B132" s="24" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D132" s="12" t="n">
         <v>0</v>
@@ -8042,13 +8086,13 @@
     </row>
     <row r="133" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="50" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B133" s="24" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D133" s="12" t="n">
         <v>1</v>
@@ -8088,13 +8132,13 @@
     </row>
     <row r="134" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="50" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B134" s="24" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="D134" s="12" t="n">
         <v>0</v>
@@ -8130,13 +8174,13 @@
     </row>
     <row r="135" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="50" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B135" s="24" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D135" s="12" t="n">
         <v>1</v>
@@ -8200,13 +8244,13 @@
     </row>
     <row r="137" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="22" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B137" s="24" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D137" s="12" t="n">
         <v>1</v>
@@ -8246,13 +8290,13 @@
     </row>
     <row r="138" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="22" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B138" s="24" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D138" s="12" t="n">
         <v>1</v>
@@ -8316,10 +8360,10 @@
     </row>
     <row r="140" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="16" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B140" s="24" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="51" t="n">
@@ -8360,13 +8404,13 @@
     </row>
     <row r="141" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="16" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B141" s="24" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D141" s="12" t="n">
         <v>1</v>
@@ -8406,13 +8450,13 @@
     </row>
     <row r="142" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="16" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B142" s="24" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D142" s="12" t="n">
         <v>1</v>
@@ -8452,13 +8496,13 @@
     </row>
     <row r="143" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="16" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B143" s="24" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D143" s="12" t="n">
         <v>0</v>
@@ -8498,13 +8542,13 @@
     </row>
     <row r="144" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="16" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B144" s="24" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C144" s="34" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="D144" s="12" t="n">
         <v>0</v>
@@ -8544,13 +8588,13 @@
     </row>
     <row r="145" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="16" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B145" s="24" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D145" s="12" t="n">
         <v>0</v>
@@ -8590,13 +8634,13 @@
     </row>
     <row r="146" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="16" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B146" s="24" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D146" s="12" t="n">
         <v>0</v>
@@ -8660,13 +8704,13 @@
     </row>
     <row r="148" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B148" s="24" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D148" s="51" t="n">
         <v>1</v>
@@ -8706,13 +8750,13 @@
     </row>
     <row r="149" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B149" s="24" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D149" s="12" t="n">
         <v>1</v>
@@ -8752,13 +8796,13 @@
     </row>
     <row r="150" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B150" s="24" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D150" s="51" t="n">
         <v>1</v>
@@ -8798,13 +8842,13 @@
     </row>
     <row r="151" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B151" s="24" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D151" s="51" t="n">
         <v>1</v>
@@ -8844,13 +8888,13 @@
     </row>
     <row r="152" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B152" s="24" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D152" s="51" t="n">
         <v>1</v>
@@ -8890,13 +8934,13 @@
     </row>
     <row r="153" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B153" s="24" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D153" s="12" t="n">
         <v>1</v>
@@ -8936,13 +8980,13 @@
     </row>
     <row r="154" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B154" s="24" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D154" s="51" t="n">
         <v>1</v>
@@ -8982,13 +9026,13 @@
     </row>
     <row r="155" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B155" s="24" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D155" s="51" t="n">
         <v>1</v>
@@ -9028,13 +9072,13 @@
     </row>
     <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B156" s="24" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D156" s="12" t="n">
         <v>1</v>
@@ -9074,13 +9118,13 @@
     </row>
     <row r="157" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B157" s="24" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D157" s="12" t="n">
         <v>0</v>
@@ -9120,13 +9164,13 @@
     </row>
     <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B158" s="24" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D158" s="12" t="n">
         <v>0</v>
@@ -9166,13 +9210,13 @@
     </row>
     <row r="159" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B159" s="24" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D159" s="51" t="n">
         <v>1</v>
@@ -9236,13 +9280,13 @@
     </row>
     <row r="161" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="24" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B161" s="24" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="D161" s="12"/>
       <c r="E161" s="13"/>
@@ -9274,13 +9318,13 @@
     </row>
     <row r="162" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="24" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B162" s="24" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D162" s="12" t="n">
         <v>0</v>
@@ -9320,13 +9364,13 @@
     </row>
     <row r="163" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="24" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B163" s="24" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D163" s="12" t="n">
         <v>0</v>
@@ -9366,13 +9410,13 @@
     </row>
     <row r="164" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="24" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B164" s="24" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D164" s="12" t="n">
         <v>1</v>
@@ -9436,13 +9480,13 @@
     </row>
     <row r="166" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="24" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B166" s="24" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D166" s="12" t="n">
         <v>0</v>
@@ -10237,17 +10281,17 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="1" sqref="A27:A33 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="11" min="4" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="21" min="12" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10297,13 +10341,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="64" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C2" s="66" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="D2" s="67" t="n">
         <v>1</v>
@@ -10426,7 +10470,7 @@
       <c r="A5" s="64"/>
       <c r="B5" s="65"/>
       <c r="C5" s="66" t="s">
-        <v>17</v>
+        <v>250</v>
       </c>
       <c r="D5" s="67" t="n">
         <v>1</v>
@@ -10467,7 +10511,7 @@
       <c r="A6" s="64"/>
       <c r="B6" s="65"/>
       <c r="C6" s="66" t="s">
-        <v>18</v>
+        <v>251</v>
       </c>
       <c r="D6" s="67" t="n">
         <v>1</v>
@@ -10584,7 +10628,7 @@
       <c r="A9" s="64"/>
       <c r="B9" s="65"/>
       <c r="C9" s="66" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="67" t="n">
         <v>1</v>
@@ -10625,7 +10669,7 @@
       <c r="A10" s="64"/>
       <c r="B10" s="65"/>
       <c r="C10" s="66" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" s="67"/>
       <c r="E10" s="68"/>
@@ -10660,7 +10704,7 @@
       <c r="A11" s="64"/>
       <c r="B11" s="65"/>
       <c r="C11" s="66" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D11" s="67" t="n">
         <v>1</v>
@@ -10699,7 +10743,7 @@
       <c r="A12" s="71"/>
       <c r="B12" s="72"/>
       <c r="C12" s="73" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D12" s="74"/>
       <c r="E12" s="75" t="n">
@@ -10734,7 +10778,7 @@
       <c r="A13" s="78"/>
       <c r="B13" s="72"/>
       <c r="C13" s="79" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="D13" s="74"/>
       <c r="E13" s="75"/>
@@ -10759,7 +10803,7 @@
       <c r="A14" s="78"/>
       <c r="B14" s="72"/>
       <c r="C14" s="79" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="D14" s="74"/>
       <c r="E14" s="75"/>
@@ -10783,7 +10827,7 @@
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="64"/>
       <c r="B15" s="65" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" s="66"/>
       <c r="D15" s="67" t="n">
@@ -10816,10 +10860,10 @@
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="64"/>
       <c r="B16" s="81" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C16" s="66" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="D16" s="67"/>
       <c r="E16" s="68" t="n">
@@ -10853,10 +10897,10 @@
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="64"/>
       <c r="B17" s="65" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C17" s="66" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D17" s="67"/>
       <c r="E17" s="68" t="n">
@@ -10890,10 +10934,10 @@
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="78"/>
       <c r="B18" s="72" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C18" s="80" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D18" s="74" t="n">
         <v>1</v>
@@ -10923,10 +10967,10 @@
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="71"/>
       <c r="B19" s="72" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C19" s="73" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="D19" s="67" t="n">
         <v>1</v>
@@ -10978,13 +11022,13 @@
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="78" t="s">
-        <v>35</v>
+        <v>260</v>
       </c>
       <c r="B21" s="81" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C21" s="66" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D21" s="67" t="n">
         <v>1</v>
@@ -11020,7 +11064,7 @@
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="78"/>
       <c r="B22" s="81" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="C22" s="66"/>
       <c r="D22" s="67"/>
@@ -11055,10 +11099,10 @@
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="78"/>
       <c r="B23" s="72" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="C23" s="66" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="D23" s="67"/>
       <c r="E23" s="68" t="n">
@@ -11110,10 +11154,10 @@
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="64" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="B25" s="72" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="C25" s="66"/>
       <c r="D25" s="67" t="n">
@@ -11146,7 +11190,7 @@
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="64"/>
       <c r="B26" s="72" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="C26" s="66"/>
       <c r="D26" s="67" t="n">
@@ -11181,7 +11225,7 @@
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="64"/>
       <c r="B27" s="72" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C27" s="66"/>
       <c r="D27" s="67" t="n">
@@ -11216,7 +11260,7 @@
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="64"/>
       <c r="B28" s="72" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="C28" s="66"/>
       <c r="D28" s="67" t="n">
@@ -11251,7 +11295,7 @@
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="64"/>
       <c r="B29" s="72" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="C29" s="66"/>
       <c r="D29" s="67" t="n">
@@ -11286,7 +11330,7 @@
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="64"/>
       <c r="B30" s="72" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="C30" s="66"/>
       <c r="D30" s="67" t="n">
@@ -11321,7 +11365,7 @@
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="64"/>
       <c r="B31" s="72" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C31" s="66"/>
       <c r="D31" s="67" t="n">
@@ -11378,13 +11422,13 @@
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="93" t="s">
-        <v>56</v>
+        <v>274</v>
       </c>
       <c r="B33" s="94" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="C33" s="88" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="D33" s="89" t="n">
         <v>1</v>
@@ -11420,10 +11464,10 @@
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="93"/>
       <c r="B34" s="82" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="C34" s="88" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="D34" s="89" t="n">
         <v>1</v>
@@ -11481,13 +11525,13 @@
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="64" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C36" s="66" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D36" s="67" t="n">
         <v>1</v>
@@ -11523,10 +11567,10 @@
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="64"/>
       <c r="B37" s="65" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C37" s="66" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="D37" s="67"/>
       <c r="E37" s="68" t="n">
@@ -11560,10 +11604,10 @@
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="71"/>
       <c r="B38" s="65" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C38" s="66" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D38" s="67" t="n">
         <v>1</v>
@@ -11599,10 +11643,10 @@
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="64"/>
       <c r="B39" s="95" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C39" s="66" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="D39" s="67" t="n">
         <v>1</v>
@@ -11638,10 +11682,10 @@
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="64"/>
       <c r="B40" s="65" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C40" s="66" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="D40" s="67" t="n">
         <v>1</v>
@@ -11675,7 +11719,7 @@
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="64"/>
       <c r="B41" s="65" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C41" s="66"/>
       <c r="D41" s="67" t="n">
@@ -11710,7 +11754,7 @@
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="64"/>
       <c r="B42" s="65" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="C42" s="66"/>
       <c r="D42" s="67"/>
@@ -11743,7 +11787,7 @@
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="64"/>
       <c r="B43" s="65" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C43" s="66"/>
       <c r="D43" s="67"/>
@@ -11776,10 +11820,10 @@
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="64"/>
       <c r="B44" s="65" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C44" s="66" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="D44" s="67"/>
       <c r="E44" s="68"/>
@@ -11811,10 +11855,10 @@
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="64"/>
       <c r="B45" s="65" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C45" s="66" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="D45" s="67"/>
       <c r="E45" s="68"/>
@@ -11891,13 +11935,13 @@
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="93" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B48" s="96" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="C48" s="88" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="D48" s="89" t="n">
         <v>1</v>
@@ -11927,10 +11971,10 @@
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="87"/>
       <c r="B49" s="96" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="C49" s="97" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="D49" s="89" t="n">
         <v>1</v>
@@ -11960,10 +12004,10 @@
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="87"/>
       <c r="B50" s="96" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="C50" s="97" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="D50" s="89" t="n">
         <v>1</v>
@@ -11993,10 +12037,10 @@
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="87"/>
       <c r="B51" s="94" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="C51" s="98" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D51" s="89"/>
       <c r="E51" s="90"/>
@@ -12024,10 +12068,10 @@
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="93"/>
       <c r="B52" s="94" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="C52" s="88" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="D52" s="89" t="n">
         <v>1</v>
@@ -12063,10 +12107,10 @@
     <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="93"/>
       <c r="B53" s="94" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C53" s="88" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="D53" s="89"/>
       <c r="E53" s="90"/>
@@ -12098,10 +12142,10 @@
     <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="93"/>
       <c r="B54" s="99" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C54" s="88" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D54" s="89" t="n">
         <v>1</v>
@@ -12138,7 +12182,7 @@
       <c r="A55" s="93"/>
       <c r="B55" s="82"/>
       <c r="C55" s="88" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D55" s="89"/>
       <c r="E55" s="90"/>
@@ -12170,10 +12214,10 @@
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="93"/>
       <c r="B56" s="99" t="s">
+        <v>300</v>
+      </c>
+      <c r="C56" s="100" t="s">
         <v>292</v>
-      </c>
-      <c r="C56" s="100" t="s">
-        <v>284</v>
       </c>
       <c r="D56" s="89" t="n">
         <v>1</v>
@@ -12205,7 +12249,7 @@
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="93"/>
       <c r="B57" s="82" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="C57" s="100"/>
       <c r="D57" s="89"/>
@@ -12240,7 +12284,7 @@
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="93"/>
       <c r="B58" s="82" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="C58" s="100"/>
       <c r="D58" s="89" t="n">
@@ -12277,7 +12321,7 @@
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="93"/>
       <c r="B59" s="82" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="C59" s="100"/>
       <c r="D59" s="89"/>
@@ -12310,7 +12354,7 @@
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="93"/>
       <c r="B60" s="82" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="C60" s="100"/>
       <c r="D60" s="89"/>
@@ -12365,10 +12409,10 @@
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="64" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="B62" s="72" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C62" s="101"/>
       <c r="D62" s="67" t="n">
@@ -12405,7 +12449,7 @@
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="64"/>
       <c r="B63" s="72" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="C63" s="101"/>
       <c r="D63" s="67"/>
@@ -12438,7 +12482,7 @@
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="64"/>
       <c r="B64" s="72" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="C64" s="101"/>
       <c r="D64" s="67"/>
@@ -12473,7 +12517,7 @@
     <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="64"/>
       <c r="B65" s="72" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="C65" s="101"/>
       <c r="D65" s="67"/>
@@ -12506,7 +12550,7 @@
     <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="64"/>
       <c r="B66" s="72" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="C66" s="101"/>
       <c r="D66" s="67" t="n">
@@ -12541,7 +12585,7 @@
     <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="64"/>
       <c r="B67" s="72" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="C67" s="101"/>
       <c r="D67" s="67"/>
@@ -12574,7 +12618,7 @@
     <row r="68" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="64"/>
       <c r="B68" s="72" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="C68" s="101"/>
       <c r="D68" s="67"/>
@@ -12607,10 +12651,10 @@
     <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="64"/>
       <c r="B69" s="72" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C69" s="102" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="D69" s="67"/>
       <c r="E69" s="68" t="n">
@@ -12644,7 +12688,7 @@
     <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="64"/>
       <c r="B70" s="72" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="C70" s="101"/>
       <c r="D70" s="67" t="n">
@@ -12681,7 +12725,7 @@
     <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="64"/>
       <c r="B71" s="103" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="C71" s="101"/>
       <c r="D71" s="67"/>
@@ -12706,7 +12750,7 @@
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="104"/>
       <c r="B72" s="105" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="C72" s="106"/>
       <c r="D72" s="107"/>
@@ -12731,7 +12775,7 @@
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="64"/>
       <c r="B73" s="103" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="C73" s="101"/>
       <c r="D73" s="67"/>
@@ -12755,13 +12799,13 @@
     </row>
     <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="93" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B74" s="94" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="C74" s="88" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="D74" s="89" t="n">
         <v>1</v>
@@ -12801,10 +12845,10 @@
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="93"/>
       <c r="B75" s="94" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="C75" s="112" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="D75" s="89"/>
       <c r="E75" s="90"/>
@@ -12836,10 +12880,10 @@
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="93"/>
       <c r="B76" s="94" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C76" s="88" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="D76" s="89" t="n">
         <v>1</v>
@@ -12875,10 +12919,10 @@
     <row r="77" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="93"/>
       <c r="B77" s="94" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="C77" s="88" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="D77" s="89" t="n">
         <v>1</v>
@@ -12914,10 +12958,10 @@
     <row r="78" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="93"/>
       <c r="B78" s="94" t="s">
-        <v>126</v>
+        <v>327</v>
       </c>
       <c r="C78" s="88" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="D78" s="89"/>
       <c r="E78" s="90" t="n">
@@ -12951,10 +12995,10 @@
     <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="3"/>
       <c r="B79" s="99" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C79" s="34" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="D79" s="83" t="n">
         <v>1</v>
@@ -12990,7 +13034,7 @@
     <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="3"/>
       <c r="B80" s="99" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="C80" s="34"/>
       <c r="D80" s="83" t="n">
@@ -13027,10 +13071,10 @@
     <row r="81" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="3"/>
       <c r="B81" s="99" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="C81" s="34" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="D81" s="83" t="n">
         <v>1</v>
@@ -13060,10 +13104,10 @@
     <row r="82" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>
       <c r="B82" s="99" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C82" s="100" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="D82" s="83" t="n">
         <v>1</v>
@@ -13095,10 +13139,10 @@
     <row r="83" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="93"/>
       <c r="B83" s="113" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="C83" s="100" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="D83" s="83" t="n">
         <v>1</v>
@@ -13130,7 +13174,7 @@
     <row r="84" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="93"/>
       <c r="B84" s="82" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C84" s="100"/>
       <c r="D84" s="83"/>
@@ -13159,7 +13203,7 @@
     <row r="85" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="93"/>
       <c r="B85" s="82" t="s">
-        <v>135</v>
+        <v>336</v>
       </c>
       <c r="C85" s="100"/>
       <c r="D85" s="83"/>
@@ -13186,10 +13230,10 @@
     <row r="86" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="93"/>
       <c r="B86" s="82" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C86" s="100" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D86" s="83"/>
       <c r="E86" s="84"/>
@@ -13217,10 +13261,10 @@
     <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="93"/>
       <c r="B87" s="82" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C87" s="100" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D87" s="83"/>
       <c r="E87" s="84"/>
@@ -13246,7 +13290,7 @@
     <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="93"/>
       <c r="B88" s="82" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="C88" s="100"/>
       <c r="D88" s="83"/>
@@ -13297,13 +13341,13 @@
     </row>
     <row r="90" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="93" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="B90" s="94" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="C90" s="88" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="D90" s="83"/>
       <c r="E90" s="90" t="n">
@@ -13337,7 +13381,7 @@
     <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="93"/>
       <c r="B91" s="94" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="C91" s="34"/>
       <c r="D91" s="89"/>
@@ -13372,7 +13416,7 @@
     <row r="92" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="93"/>
       <c r="B92" s="94" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C92" s="88"/>
       <c r="D92" s="89"/>
@@ -13407,10 +13451,10 @@
     <row r="93" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="93"/>
       <c r="B93" s="94" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C93" s="88" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="D93" s="89"/>
       <c r="E93" s="90" t="n">
@@ -13466,10 +13510,10 @@
     </row>
     <row r="95" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="93" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="B95" s="94" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="C95" s="88"/>
       <c r="D95" s="89"/>
@@ -13504,7 +13548,7 @@
     <row r="96" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="93"/>
       <c r="B96" s="94" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C96" s="88"/>
       <c r="D96" s="89"/>
@@ -13539,7 +13583,7 @@
     <row r="97" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="93"/>
       <c r="B97" s="94" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="C97" s="88"/>
       <c r="D97" s="89" t="n">
@@ -13576,7 +13620,7 @@
     <row r="98" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="93"/>
       <c r="B98" s="94" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="C98" s="88"/>
       <c r="D98" s="89"/>
@@ -13633,11 +13677,11 @@
     </row>
     <row r="100" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="87" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="B100" s="82"/>
       <c r="C100" s="34" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="D100" s="89"/>
       <c r="E100" s="90"/>
@@ -13687,13 +13731,13 @@
     </row>
     <row r="102" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="87" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B102" s="82" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C102" s="100" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="D102" s="89"/>
       <c r="E102" s="90"/>
@@ -13725,10 +13769,10 @@
     <row r="103" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="3"/>
       <c r="B103" s="82" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="C103" s="100" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="D103" s="89"/>
       <c r="E103" s="90" t="n">
@@ -13784,13 +13828,13 @@
     </row>
     <row r="105" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="B105" s="99" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="C105" s="88" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D105" s="89"/>
       <c r="E105" s="90" t="n">
@@ -13824,10 +13868,10 @@
     <row r="106" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="3"/>
       <c r="B106" s="99" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="C106" s="88" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D106" s="89" t="n">
         <v>1</v>
@@ -13864,7 +13908,7 @@
       <c r="A107" s="3"/>
       <c r="B107" s="99"/>
       <c r="C107" s="88" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D107" s="89"/>
       <c r="E107" s="90" t="n">
@@ -13899,7 +13943,7 @@
       <c r="A108" s="3"/>
       <c r="B108" s="99"/>
       <c r="C108" s="88" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D108" s="89"/>
       <c r="E108" s="90"/>
@@ -13932,7 +13976,7 @@
       <c r="A109" s="3"/>
       <c r="B109" s="99"/>
       <c r="C109" s="88" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D109" s="89"/>
       <c r="E109" s="90" t="n">
@@ -13967,7 +14011,7 @@
       <c r="A110" s="3"/>
       <c r="B110" s="99"/>
       <c r="C110" s="88" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="D110" s="89" t="n">
         <v>1</v>
@@ -14002,7 +14046,7 @@
       <c r="A111" s="3"/>
       <c r="B111" s="99"/>
       <c r="C111" s="88" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D111" s="89" t="n">
         <v>1</v>
@@ -14037,7 +14081,7 @@
       <c r="A112" s="3"/>
       <c r="B112" s="99"/>
       <c r="C112" s="88" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D112" s="89"/>
       <c r="E112" s="90" t="n">
@@ -14072,7 +14116,7 @@
       <c r="A113" s="3"/>
       <c r="B113" s="99"/>
       <c r="C113" s="88" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D113" s="89"/>
       <c r="E113" s="90"/>
@@ -14105,7 +14149,7 @@
       <c r="A114" s="3"/>
       <c r="B114" s="82"/>
       <c r="C114" s="88" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D114" s="89"/>
       <c r="E114" s="90"/>
@@ -14138,7 +14182,7 @@
       <c r="A115" s="3"/>
       <c r="B115" s="82"/>
       <c r="C115" s="100" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D115" s="89" t="n">
         <v>1</v>
@@ -14175,7 +14219,7 @@
       <c r="A116" s="3"/>
       <c r="B116" s="99"/>
       <c r="C116" s="88" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D116" s="89" t="n">
         <v>1</v>
@@ -14210,7 +14254,7 @@
       <c r="A117" s="3"/>
       <c r="B117" s="99"/>
       <c r="C117" s="88" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D117" s="89"/>
       <c r="E117" s="84"/>
@@ -14242,10 +14286,10 @@
     <row r="118" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="3"/>
       <c r="B118" s="93" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="C118" s="100" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="D118" s="89" t="n">
         <v>1</v>
@@ -14275,10 +14319,10 @@
     <row r="119" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="3"/>
       <c r="B119" s="99" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="C119" s="88" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D119" s="89" t="n">
         <v>1</v>
@@ -14308,10 +14352,10 @@
     <row r="120" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="3"/>
       <c r="B120" s="99" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="C120" s="88" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="D120" s="89" t="n">
         <v>1</v>
@@ -14341,10 +14385,10 @@
     <row r="121" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="3"/>
       <c r="B121" s="99" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="C121" s="88" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="D121" s="89" t="n">
         <v>1</v>
@@ -14374,10 +14418,10 @@
     <row r="122" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="3"/>
       <c r="B122" s="99" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="C122" s="88" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="D122" s="89" t="n">
         <v>1</v>
@@ -14407,10 +14451,10 @@
     <row r="123" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="3"/>
       <c r="B123" s="99" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="C123" s="88" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="D123" s="89" t="n">
         <v>1</v>
@@ -14440,7 +14484,7 @@
     <row r="124" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="3"/>
       <c r="B124" s="99" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="C124" s="88"/>
       <c r="D124" s="89"/>
@@ -14475,10 +14519,10 @@
     <row r="125" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="3"/>
       <c r="B125" s="99" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="C125" s="88" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="D125" s="89" t="n">
         <v>1</v>
@@ -14514,10 +14558,10 @@
     <row r="126" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="3"/>
       <c r="B126" s="99" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="C126" s="88" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D126" s="89" t="n">
         <v>1</v>
@@ -14553,7 +14597,7 @@
     <row r="127" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="3"/>
       <c r="B127" s="99" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C127" s="34"/>
       <c r="D127" s="89"/>
@@ -14586,7 +14630,7 @@
     <row r="128" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="3"/>
       <c r="B128" s="82" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="C128" s="34"/>
       <c r="D128" s="89"/>
@@ -14639,31 +14683,31 @@
     </row>
     <row r="130" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="71" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B130" s="72" t="s">
-        <v>185</v>
+        <v>375</v>
       </c>
       <c r="C130" s="66" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="D130" s="67" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="E130" s="68" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="F130" s="69" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="G130" s="70" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="H130" s="64" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="I130" s="66" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="J130" s="66"/>
       <c r="K130" s="66"/>
@@ -14681,10 +14725,10 @@
     <row r="131" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="114"/>
       <c r="B131" s="115" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C131" s="116" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="D131" s="117" t="n">
         <v>1</v>
@@ -14742,11 +14786,11 @@
     </row>
     <row r="133" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="B133" s="82"/>
       <c r="C133" s="88" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="D133" s="89"/>
       <c r="E133" s="90"/>
@@ -14775,13 +14819,13 @@
     </row>
     <row r="134" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="71" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="B134" s="72" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C134" s="73" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="D134" s="74"/>
       <c r="E134" s="68"/>
@@ -14813,10 +14857,10 @@
     <row r="135" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="64"/>
       <c r="B135" s="65" t="s">
-        <v>374</v>
+        <v>385</v>
       </c>
       <c r="C135" s="66" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="D135" s="67"/>
       <c r="E135" s="68" t="n">
@@ -14846,10 +14890,10 @@
     <row r="136" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="64"/>
       <c r="B136" s="65" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C136" s="66" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="D136" s="67" t="n">
         <v>1</v>
@@ -14883,10 +14927,10 @@
     <row r="137" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="71"/>
       <c r="B137" s="65" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="C137" s="73" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
       <c r="D137" s="74"/>
       <c r="E137" s="68" t="n">
@@ -14918,7 +14962,7 @@
     <row r="138" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="3"/>
       <c r="B138" s="82" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="C138" s="34"/>
       <c r="D138" s="83" t="n">
@@ -14928,10 +14972,10 @@
         <v>0</v>
       </c>
       <c r="F138" s="91" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="G138" s="92" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="H138" s="93" t="n">
         <v>1</v>
@@ -14977,13 +15021,13 @@
     </row>
     <row r="140" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="71" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B140" s="72" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="C140" s="73" t="s">
-        <v>381</v>
+        <v>392</v>
       </c>
       <c r="D140" s="74" t="n">
         <v>1</v>
@@ -15019,10 +15063,10 @@
     <row r="141" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="93"/>
       <c r="B141" s="94" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C141" s="88" t="s">
-        <v>382</v>
+        <v>393</v>
       </c>
       <c r="D141" s="89" t="n">
         <v>1</v>
@@ -15080,10 +15124,10 @@
     </row>
     <row r="143" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="B143" s="82" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="C143" s="34"/>
       <c r="D143" s="83" t="n">
@@ -15142,10 +15186,10 @@
     </row>
     <row r="145" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="88" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="B145" s="94" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="C145" s="88"/>
       <c r="D145" s="123"/>
@@ -15176,10 +15220,10 @@
     <row r="146" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="64"/>
       <c r="B146" s="65" t="s">
-        <v>387</v>
+        <v>398</v>
       </c>
       <c r="C146" s="66" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="D146" s="67" t="n">
         <v>1</v>
@@ -15215,10 +15259,10 @@
     <row r="147" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="64"/>
       <c r="B147" s="65" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
       <c r="C147" s="66" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="D147" s="67" t="n">
         <v>1</v>
@@ -15248,7 +15292,7 @@
     <row r="148" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="64"/>
       <c r="B148" s="65" t="s">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="C148" s="66"/>
       <c r="D148" s="67"/>
@@ -15283,10 +15327,10 @@
     <row r="149" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="64"/>
       <c r="B149" s="65" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="C149" s="66" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="D149" s="67"/>
       <c r="E149" s="68"/>
@@ -15318,7 +15362,7 @@
     <row r="150" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="64"/>
       <c r="B150" s="65" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
       <c r="C150" s="66"/>
       <c r="D150" s="67"/>
@@ -15351,7 +15395,7 @@
     <row r="151" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="93"/>
       <c r="B151" s="94" t="s">
-        <v>395</v>
+        <v>406</v>
       </c>
       <c r="C151" s="88"/>
       <c r="D151" s="89"/>
@@ -15404,10 +15448,10 @@
     </row>
     <row r="153" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="93" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="B153" s="94" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="C153" s="88"/>
       <c r="D153" s="89"/>
@@ -15440,7 +15484,7 @@
     <row r="154" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="93"/>
       <c r="B154" s="94" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="C154" s="88"/>
       <c r="D154" s="89"/>
@@ -15495,14 +15539,14 @@
     </row>
     <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="66" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="B156" s="65" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="C156" s="66"/>
       <c r="D156" s="127" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="E156" s="128" t="n">
         <v>3285</v>
@@ -15511,13 +15555,13 @@
         <v>518</v>
       </c>
       <c r="G156" s="130" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="H156" s="131" t="n">
         <v>635</v>
       </c>
       <c r="I156" s="66" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="J156" s="66"/>
       <c r="K156" s="66"/>
@@ -15534,10 +15578,10 @@
     </row>
     <row r="157" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="66" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="B157" s="65" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="C157" s="66"/>
       <c r="D157" s="132" t="n">
@@ -15548,13 +15592,13 @@
         <v>1295</v>
       </c>
       <c r="G157" s="130" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="H157" s="133" t="n">
         <v>852</v>
       </c>
       <c r="I157" s="66" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="J157" s="66" t="n">
         <v>875</v>
@@ -15576,10 +15620,10 @@
     </row>
     <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="134" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="B158" s="65" t="s">
-        <v>407</v>
+        <v>418</v>
       </c>
       <c r="C158" s="66"/>
       <c r="D158" s="135" t="n">
@@ -15590,13 +15634,13 @@
         <v>625</v>
       </c>
       <c r="G158" s="130" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="H158" s="133" t="n">
         <v>317.5</v>
       </c>
       <c r="I158" s="66" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="J158" s="66"/>
       <c r="K158" s="66"/>
@@ -15613,10 +15657,10 @@
     </row>
     <row r="159" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="66" t="s">
-        <v>408</v>
+        <v>419</v>
       </c>
       <c r="B159" s="65" t="s">
-        <v>409</v>
+        <v>420</v>
       </c>
       <c r="C159" s="66"/>
       <c r="D159" s="127" t="n">
@@ -15629,13 +15673,13 @@
         <v>30</v>
       </c>
       <c r="G159" s="130" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="H159" s="66" t="n">
         <v>14</v>
       </c>
       <c r="I159" s="66" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
       <c r="J159" s="66"/>
       <c r="K159" s="66"/>
@@ -15652,17 +15696,17 @@
     </row>
     <row r="160" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="66" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
       <c r="B160" s="65" t="s">
-        <v>412</v>
+        <v>423</v>
       </c>
       <c r="C160" s="66" t="s">
-        <v>413</v>
+        <v>424</v>
       </c>
       <c r="D160" s="127"/>
       <c r="E160" s="137" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="F160" s="138" t="n">
         <v>0</v>
@@ -15688,10 +15732,10 @@
     <row r="161" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="66"/>
       <c r="B161" s="65" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
       <c r="C161" s="66" t="s">
-        <v>416</v>
+        <v>427</v>
       </c>
       <c r="D161" s="127"/>
       <c r="E161" s="137" t="n">
@@ -15722,7 +15766,7 @@
       <c r="A162" s="66"/>
       <c r="B162" s="65"/>
       <c r="C162" s="66" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="D162" s="127"/>
       <c r="E162" s="137" t="n">
@@ -15753,7 +15797,7 @@
       <c r="A163" s="66"/>
       <c r="B163" s="65"/>
       <c r="C163" s="66" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="D163" s="127"/>
       <c r="E163" s="137"/>
@@ -15782,7 +15826,7 @@
       <c r="A164" s="66"/>
       <c r="B164" s="65"/>
       <c r="C164" s="66" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="D164" s="127"/>
       <c r="E164" s="137"/>
@@ -15811,7 +15855,7 @@
       <c r="A165" s="66"/>
       <c r="B165" s="65"/>
       <c r="C165" s="66" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="D165" s="127"/>
       <c r="E165" s="137"/>
@@ -15840,7 +15884,7 @@
       <c r="A166" s="66"/>
       <c r="B166" s="65"/>
       <c r="C166" s="66" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="D166" s="127"/>
       <c r="E166" s="137"/>
@@ -15890,27 +15934,27 @@
     </row>
     <row r="168" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="88" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B168" s="94"/>
       <c r="C168" s="88"/>
       <c r="D168" s="123" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="E168" s="124" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="F168" s="125" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="G168" s="126" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="H168" s="88" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="I168" s="88" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="J168" s="88"/>
       <c r="K168" s="88"/>
@@ -15927,7 +15971,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="94" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C169" s="88"/>
       <c r="D169" s="123" t="n">
@@ -15962,10 +16006,10 @@
     <row r="170" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="93"/>
       <c r="B170" s="94" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C170" s="88" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D170" s="89" t="n">
         <v>1</v>
@@ -15999,7 +16043,7 @@
     <row r="171" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="88"/>
       <c r="B171" s="94" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C171" s="88"/>
       <c r="D171" s="123" t="n">
@@ -16034,7 +16078,7 @@
     <row r="172" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="88"/>
       <c r="B172" s="94" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C172" s="88"/>
       <c r="D172" s="123" t="n">
@@ -16069,7 +16113,7 @@
     <row r="173" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="88"/>
       <c r="B173" s="94" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="C173" s="88"/>
       <c r="D173" s="123" t="n">
@@ -16106,10 +16150,10 @@
     <row r="174" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="93"/>
       <c r="B174" s="94" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C174" s="88" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D174" s="89" t="n">
         <v>1</v>
@@ -16145,7 +16189,7 @@
     <row r="175" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="88"/>
       <c r="B175" s="94" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="C175" s="88"/>
       <c r="D175" s="123" t="n">
@@ -16182,10 +16226,10 @@
     <row r="176" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="88"/>
       <c r="B176" s="94" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="C176" s="88" t="s">
-        <v>425</v>
+        <v>436</v>
       </c>
       <c r="D176" s="123" t="n">
         <v>1</v>
@@ -16221,10 +16265,10 @@
     <row r="177" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="88"/>
       <c r="B177" s="94" t="s">
-        <v>426</v>
+        <v>437</v>
       </c>
       <c r="C177" s="88" t="s">
-        <v>427</v>
+        <v>438</v>
       </c>
       <c r="D177" s="123"/>
       <c r="E177" s="124" t="n">
@@ -16258,10 +16302,10 @@
     <row r="178" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="93"/>
       <c r="B178" s="94" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C178" s="88" t="s">
-        <v>428</v>
+        <v>439</v>
       </c>
       <c r="D178" s="89" t="n">
         <v>1</v>
@@ -16297,10 +16341,10 @@
     <row r="179" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="93"/>
       <c r="B179" s="94" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C179" s="88" t="s">
-        <v>429</v>
+        <v>440</v>
       </c>
       <c r="D179" s="89"/>
       <c r="E179" s="90" t="n">
@@ -16334,10 +16378,10 @@
     <row r="180" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="93"/>
       <c r="B180" s="94" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C180" s="88" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D180" s="89"/>
       <c r="E180" s="90" t="n">
@@ -16371,10 +16415,10 @@
     <row r="181" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="88"/>
       <c r="B181" s="94" t="s">
-        <v>232</v>
+        <v>441</v>
       </c>
       <c r="C181" s="88" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="D181" s="123" t="n">
         <v>1</v>
@@ -16432,10 +16476,10 @@
     </row>
     <row r="183" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="94" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B183" s="94" t="s">
-        <v>235</v>
+        <v>443</v>
       </c>
       <c r="C183" s="88"/>
       <c r="D183" s="89"/>
@@ -16464,7 +16508,7 @@
     <row r="184" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="94"/>
       <c r="B184" s="94" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C184" s="88"/>
       <c r="D184" s="89"/>
@@ -16493,7 +16537,7 @@
     <row r="185" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="94"/>
       <c r="B185" s="94" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C185" s="88"/>
       <c r="D185" s="89"/>
@@ -16522,7 +16566,7 @@
     <row r="186" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="94"/>
       <c r="B186" s="94" t="s">
-        <v>239</v>
+        <v>444</v>
       </c>
       <c r="C186" s="88"/>
       <c r="D186" s="89"/>
@@ -16573,10 +16617,10 @@
     </row>
     <row r="188" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="94" t="s">
-        <v>431</v>
+        <v>445</v>
       </c>
       <c r="B188" s="94" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
       <c r="C188" s="88"/>
       <c r="D188" s="89"/>
@@ -16609,7 +16653,7 @@
     <row r="189" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="140"/>
       <c r="B189" s="94" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C189" s="88"/>
       <c r="D189" s="89"/>

</xml_diff>